<commit_message>
Deploying to gh-pages from  @ c058db0648ef8abe7929016c93f536621f043cff 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/7.1.1.xlsx
+++ b/en/downloads/data-excel/7.1.1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
   <si>
     <t>Профессиональное высшее</t>
   </si>
@@ -74,15 +74,6 @@
     <t>Кыргызская Республика</t>
   </si>
   <si>
-    <t>2018</t>
-  </si>
-  <si>
-    <t>2017</t>
-  </si>
-  <si>
-    <t>2016</t>
-  </si>
-  <si>
     <t>(в процентах к численности населения)</t>
   </si>
   <si>
@@ -305,9 +296,6 @@
     <t>Богатейший</t>
   </si>
   <si>
-    <t>2019</t>
-  </si>
-  <si>
     <t xml:space="preserve">Жакыр </t>
   </si>
   <si>
@@ -351,9 +339,6 @@
   </si>
   <si>
     <t>(жалпы калктын санына карата пайыз менен)</t>
-  </si>
-  <si>
-    <t>2020</t>
   </si>
   <si>
     <t>Жынысы боюняа</t>
@@ -565,9 +550,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -657,6 +639,9 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -943,9 +928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -954,19 +937,19 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+    <row r="1" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
       <c r="G1" s="6"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
@@ -974,18 +957,18 @@
       <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="A2" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
       <c r="G2" s="6"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -993,60 +976,62 @@
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="5"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
     </row>
     <row r="4" spans="1:11" s="4" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="I4" s="18">
+      <c r="A4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="39">
+        <v>2016</v>
+      </c>
+      <c r="E4" s="39">
+        <v>2017</v>
+      </c>
+      <c r="F4" s="39">
+        <v>2018</v>
+      </c>
+      <c r="G4" s="39">
+        <v>2019</v>
+      </c>
+      <c r="H4" s="39">
+        <v>2020</v>
+      </c>
+      <c r="I4" s="17">
         <v>2021</v>
       </c>
-      <c r="J4" s="18">
+      <c r="J4" s="17">
         <v>2022</v>
       </c>
-      <c r="K4" s="7"/>
+      <c r="K4" s="17">
+        <v>2023</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="19" t="s">
+      <c r="A5" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>54</v>
+      <c r="C5" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="D5" s="3">
         <v>76.659489882744069</v>
@@ -1063,42 +1048,44 @@
       <c r="H5" s="3">
         <v>72.8</v>
       </c>
-      <c r="I5" s="38">
+      <c r="I5" s="37">
         <v>70.820997495469314</v>
       </c>
-      <c r="J5" s="38">
+      <c r="J5" s="37">
         <v>73.12465619195541</v>
       </c>
-      <c r="K5" s="5"/>
+      <c r="K5" s="37">
+        <v>73.212978783392558</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="25" t="s">
+      <c r="A6" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>39</v>
+      <c r="C6" s="24" t="s">
+        <v>36</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="5"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="21" t="s">
+      <c r="A7" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>40</v>
+      <c r="C7" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="D7" s="2">
         <v>86.923359481873106</v>
@@ -1115,23 +1102,25 @@
       <c r="H7" s="2">
         <v>88.5</v>
       </c>
-      <c r="I7" s="39">
+      <c r="I7" s="38">
         <v>85.966681363769055</v>
       </c>
-      <c r="J7" s="39">
+      <c r="J7" s="38">
         <v>87.988189934744582</v>
       </c>
-      <c r="K7" s="5"/>
+      <c r="K7" s="38">
+        <v>84.732329223185104</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="21" t="s">
+      <c r="A8" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="21" t="s">
-        <v>41</v>
+      <c r="C8" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="D8" s="2">
         <v>71.082282795870498</v>
@@ -1148,42 +1137,44 @@
       <c r="H8" s="2">
         <v>64</v>
       </c>
-      <c r="I8" s="39">
+      <c r="I8" s="38">
         <v>61.842862951063616</v>
       </c>
-      <c r="J8" s="39">
+      <c r="J8" s="38">
         <v>64.500592135426857</v>
       </c>
-      <c r="K8" s="5"/>
+      <c r="K8" s="38">
+        <v>66.628666020113997</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>118</v>
+      <c r="A9" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>113</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="5"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="21" t="s">
+      <c r="A10" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>42</v>
+      <c r="C10" s="20" t="s">
+        <v>39</v>
       </c>
       <c r="D10" s="2">
         <v>76.070681971380779</v>
@@ -1200,23 +1191,25 @@
       <c r="H10" s="2">
         <v>71.8</v>
       </c>
-      <c r="I10" s="39">
+      <c r="I10" s="38">
         <v>69.96676935735357</v>
       </c>
-      <c r="J10" s="39">
+      <c r="J10" s="38">
         <v>72.384400434287286</v>
       </c>
-      <c r="K10" s="5"/>
+      <c r="K10" s="38">
+        <v>72.783677442666146</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="21" t="s">
-        <v>43</v>
+      <c r="C11" s="20" t="s">
+        <v>40</v>
       </c>
       <c r="D11" s="2">
         <v>77.19358578508951</v>
@@ -1233,42 +1226,44 @@
       <c r="H11" s="2">
         <v>73.7</v>
       </c>
-      <c r="I11" s="39">
+      <c r="I11" s="38">
         <v>71.587518731036198</v>
       </c>
-      <c r="J11" s="39">
+      <c r="J11" s="38">
         <v>73.791504465487179</v>
       </c>
-      <c r="K11" s="5"/>
+      <c r="K11" s="38">
+        <v>73.603979547335769</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>85</v>
+      <c r="A12" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>82</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="5"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>58</v>
+      <c r="A13" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>55</v>
       </c>
       <c r="D13" s="2">
         <v>75.839901244625295</v>
@@ -1285,23 +1280,25 @@
       <c r="H13" s="2">
         <v>71</v>
       </c>
-      <c r="I13" s="39">
+      <c r="I13" s="38">
         <v>53.549862023786716</v>
       </c>
-      <c r="J13" s="39">
+      <c r="J13" s="38">
         <v>59.191141810770276</v>
       </c>
-      <c r="K13" s="5"/>
+      <c r="K13" s="38">
+        <v>53.190169650876342</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>60</v>
+      <c r="A14" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="D14" s="2">
         <v>76.702406370968419</v>
@@ -1318,23 +1315,25 @@
       <c r="H14" s="2">
         <v>52.6</v>
       </c>
-      <c r="I14" s="39">
+      <c r="I14" s="38">
         <v>54.307261451023159</v>
       </c>
-      <c r="J14" s="39">
+      <c r="J14" s="38">
         <v>53.615471477347356</v>
       </c>
-      <c r="K14" s="5"/>
+      <c r="K14" s="38">
+        <v>53.980425341193509</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>62</v>
+      <c r="A15" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>59</v>
       </c>
       <c r="D15" s="2">
         <v>47.347625752470435</v>
@@ -1351,23 +1350,25 @@
       <c r="H15" s="2">
         <v>48.6</v>
       </c>
-      <c r="I15" s="39">
+      <c r="I15" s="38">
         <v>53.808776705136417</v>
       </c>
-      <c r="J15" s="39">
+      <c r="J15" s="38">
         <v>46.885693434034664</v>
       </c>
-      <c r="K15" s="5"/>
+      <c r="K15" s="38">
+        <v>53.137495385924751</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>65</v>
+      <c r="A16" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>62</v>
       </c>
       <c r="D16" s="2">
         <v>77.440012232216006</v>
@@ -1384,23 +1385,25 @@
       <c r="H16" s="2">
         <v>77.400000000000006</v>
       </c>
-      <c r="I16" s="39">
+      <c r="I16" s="38">
         <v>77.926565039059156</v>
       </c>
-      <c r="J16" s="39">
+      <c r="J16" s="38">
         <v>70.904364211592579</v>
       </c>
-      <c r="K16" s="5"/>
+      <c r="K16" s="38">
+        <v>72.873094526683218</v>
+      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>68</v>
+      <c r="A17" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>65</v>
       </c>
       <c r="D17" s="2">
         <v>74.642533676215891</v>
@@ -1417,23 +1420,25 @@
       <c r="H17" s="2">
         <v>66.900000000000006</v>
       </c>
-      <c r="I17" s="39">
+      <c r="I17" s="38">
         <v>63.504823365954039</v>
       </c>
-      <c r="J17" s="39">
+      <c r="J17" s="38">
         <v>73.702360776761452</v>
       </c>
-      <c r="K17" s="5"/>
+      <c r="K17" s="38">
+        <v>85.786816943292436</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>71</v>
+      <c r="A18" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>68</v>
       </c>
       <c r="D18" s="2">
         <v>73.71869980389674</v>
@@ -1450,23 +1455,25 @@
       <c r="H18" s="2">
         <v>53.6</v>
       </c>
-      <c r="I18" s="39">
+      <c r="I18" s="38">
         <v>54.390584881065699</v>
       </c>
-      <c r="J18" s="39">
+      <c r="J18" s="38">
         <v>54.137210938390183</v>
       </c>
-      <c r="K18" s="5"/>
+      <c r="K18" s="38">
+        <v>51.070121416862371</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>74</v>
+      <c r="A19" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>71</v>
       </c>
       <c r="D19" s="2">
         <v>72.259616837688128</v>
@@ -1483,23 +1490,25 @@
       <c r="H19" s="2">
         <v>87.3</v>
       </c>
-      <c r="I19" s="39">
+      <c r="I19" s="38">
         <v>82.345361607838782</v>
       </c>
-      <c r="J19" s="39">
+      <c r="J19" s="38">
         <v>84.677527769165863</v>
       </c>
-      <c r="K19" s="5"/>
+      <c r="K19" s="38">
+        <v>74.345691705122476</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>77</v>
+      <c r="A20" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>74</v>
       </c>
       <c r="D20" s="2">
         <v>91.985988240965199</v>
@@ -1516,23 +1525,25 @@
       <c r="H20" s="2">
         <v>99.6</v>
       </c>
-      <c r="I20" s="39">
+      <c r="I20" s="38">
         <v>99.353342547882974</v>
       </c>
-      <c r="J20" s="39">
+      <c r="J20" s="38">
         <v>100</v>
       </c>
-      <c r="K20" s="5"/>
+      <c r="K20" s="38">
+        <v>95.320355478300954</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>80</v>
+      <c r="A21" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>77</v>
       </c>
       <c r="D21" s="2">
         <v>100</v>
@@ -1549,42 +1560,44 @@
       <c r="H21" s="2">
         <v>100</v>
       </c>
-      <c r="I21" s="39">
+      <c r="I21" s="38">
         <v>100</v>
       </c>
-      <c r="J21" s="39">
+      <c r="J21" s="38">
         <v>99.930852404081477</v>
       </c>
-      <c r="K21" s="5"/>
+      <c r="K21" s="38">
+        <v>99.411762689042433</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>116</v>
+      <c r="A22" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="5"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="21" t="s">
+      <c r="A23" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="21" t="s">
-        <v>44</v>
+      <c r="C23" s="20" t="s">
+        <v>41</v>
       </c>
       <c r="D23" s="2">
         <v>75.934458161033746</v>
@@ -1601,23 +1614,25 @@
       <c r="H23" s="2">
         <v>71.8</v>
       </c>
-      <c r="I23" s="39">
+      <c r="I23" s="38">
         <v>69.019711553134158</v>
       </c>
-      <c r="J23" s="39">
+      <c r="J23" s="38">
         <v>71.230600083182324</v>
       </c>
-      <c r="K23" s="5"/>
+      <c r="K23" s="38">
+        <v>72.729359607564902</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="21" t="s">
+      <c r="A24" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="21" t="s">
-        <v>45</v>
+      <c r="C24" s="20" t="s">
+        <v>42</v>
       </c>
       <c r="D24" s="2">
         <v>76.34227019945881</v>
@@ -1634,23 +1649,25 @@
       <c r="H24" s="2">
         <v>71.2</v>
       </c>
-      <c r="I24" s="39">
+      <c r="I24" s="38">
         <v>70.100724861141771</v>
       </c>
-      <c r="J24" s="39">
+      <c r="J24" s="38">
         <v>71.968838508206318</v>
       </c>
-      <c r="K24" s="5"/>
+      <c r="K24" s="38">
+        <v>71.960490863505655</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="21" t="s">
+      <c r="A25" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="21" t="s">
-        <v>46</v>
+      <c r="C25" s="20" t="s">
+        <v>43</v>
       </c>
       <c r="D25" s="2">
         <v>77.131081066600714</v>
@@ -1667,23 +1684,25 @@
       <c r="H25" s="2">
         <v>73</v>
       </c>
-      <c r="I25" s="39">
+      <c r="I25" s="38">
         <v>71.228883026518972</v>
       </c>
-      <c r="J25" s="39">
+      <c r="J25" s="38">
         <v>73.30989647008343</v>
       </c>
-      <c r="K25" s="5"/>
+      <c r="K25" s="38">
+        <v>72.296589678916334</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="B26" s="21" t="s">
+      <c r="A26" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="21" t="s">
-        <v>47</v>
+      <c r="C26" s="20" t="s">
+        <v>44</v>
       </c>
       <c r="D26" s="2">
         <v>76.831249160702569</v>
@@ -1700,23 +1719,25 @@
       <c r="H26" s="2">
         <v>74.2</v>
       </c>
-      <c r="I26" s="39">
+      <c r="I26" s="38">
         <v>71.56036322878731</v>
       </c>
-      <c r="J26" s="39">
+      <c r="J26" s="38">
         <v>74.679649880623586</v>
       </c>
-      <c r="K26" s="5"/>
+      <c r="K26" s="38">
+        <v>74.209057592343228</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="B27" s="21" t="s">
+      <c r="A27" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="21" t="s">
-        <v>48</v>
+      <c r="C27" s="20" t="s">
+        <v>45</v>
       </c>
       <c r="D27" s="2">
         <v>76.794900836839986</v>
@@ -1733,42 +1754,44 @@
       <c r="H27" s="2">
         <v>72.099999999999994</v>
       </c>
-      <c r="I27" s="39">
+      <c r="I27" s="38">
         <v>71.219799945358773</v>
       </c>
-      <c r="J27" s="39">
+      <c r="J27" s="38">
         <v>72.206087052416549</v>
       </c>
-      <c r="K27" s="5"/>
+      <c r="K27" s="38">
+        <v>74.103596638678965</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="C28" s="25" t="s">
-        <v>117</v>
+      <c r="A28" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>112</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="5"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" s="21" t="s">
+      <c r="A29" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="21" t="s">
-        <v>49</v>
+      <c r="C29" s="20" t="s">
+        <v>46</v>
       </c>
       <c r="D29" s="2">
         <v>75.216542499420527</v>
@@ -1785,23 +1808,25 @@
       <c r="H29" s="2">
         <v>71.7</v>
       </c>
-      <c r="I29" s="39">
+      <c r="I29" s="38">
         <v>70.310206444667045</v>
       </c>
-      <c r="J29" s="39">
+      <c r="J29" s="38">
         <v>71.961939074023562</v>
       </c>
-      <c r="K29" s="5"/>
+      <c r="K29" s="38">
+        <v>71.491699752852526</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="21" t="s">
+      <c r="A30" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="21" t="s">
-        <v>50</v>
+      <c r="C30" s="20" t="s">
+        <v>47</v>
       </c>
       <c r="D30" s="2">
         <v>80.225607237806585</v>
@@ -1818,23 +1843,25 @@
       <c r="H30" s="2">
         <v>73.8</v>
       </c>
-      <c r="I30" s="39">
+      <c r="I30" s="38">
         <v>70.746152139408821</v>
       </c>
-      <c r="J30" s="39">
+      <c r="J30" s="38">
         <v>74.67932773648721</v>
       </c>
-      <c r="K30" s="5"/>
+      <c r="K30" s="38">
+        <v>76.344653876851936</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" s="21" t="s">
+      <c r="A31" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="21" t="s">
-        <v>51</v>
+      <c r="C31" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="D31" s="2">
         <v>75.037157169622574</v>
@@ -1851,23 +1878,25 @@
       <c r="H31" s="2">
         <v>69.5</v>
       </c>
-      <c r="I31" s="39">
+      <c r="I31" s="38">
         <v>67.352567042310341</v>
       </c>
-      <c r="J31" s="39">
+      <c r="J31" s="38">
         <v>70.040281879112229</v>
       </c>
-      <c r="K31" s="5"/>
+      <c r="K31" s="38">
+        <v>69.783559341120238</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="21" t="s">
+      <c r="A32" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="21" t="s">
-        <v>52</v>
+      <c r="C32" s="20" t="s">
+        <v>49</v>
       </c>
       <c r="D32" s="2">
         <v>78.366259162463322</v>
@@ -1884,23 +1913,25 @@
       <c r="H32" s="2">
         <v>77.099999999999994</v>
       </c>
-      <c r="I32" s="39">
+      <c r="I32" s="38">
         <v>74.174069953484675</v>
       </c>
-      <c r="J32" s="39">
+      <c r="J32" s="38">
         <v>76.912571212797303</v>
       </c>
-      <c r="K32" s="5"/>
+      <c r="K32" s="38">
+        <v>75.182624551158781</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="21" t="s">
+      <c r="A33" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="21" t="s">
-        <v>53</v>
+      <c r="C33" s="20" t="s">
+        <v>50</v>
       </c>
       <c r="D33" s="2">
         <v>79.940305706626944</v>
@@ -1917,41 +1948,44 @@
       <c r="H33" s="2">
         <v>80.400000000000006</v>
       </c>
-      <c r="I33" s="39">
+      <c r="I33" s="38">
         <v>78.976389541746173</v>
       </c>
-      <c r="J33" s="39">
+      <c r="J33" s="38">
         <v>80.478077948570117</v>
       </c>
-      <c r="K33" s="5"/>
+      <c r="K33" s="38">
+        <v>81.728384968235133</v>
+      </c>
     </row>
     <row r="34" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="B34" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="C34" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="D34" s="28"/>
+      <c r="A34" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" s="27"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="38"/>
+      <c r="K34" s="38"/>
     </row>
     <row r="35" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="s">
-        <v>94</v>
+      <c r="A35" s="28" t="s">
+        <v>90</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C35" s="30" t="s">
-        <v>100</v>
+        <v>85</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>96</v>
       </c>
       <c r="D35" s="2">
         <v>72.459520762156927</v>
@@ -1968,22 +2002,25 @@
       <c r="H35" s="2">
         <v>66.873388076147322</v>
       </c>
-      <c r="I35" s="39">
+      <c r="I35" s="38">
         <v>64.367693980609559</v>
       </c>
-      <c r="J35" s="39">
+      <c r="J35" s="38">
         <v>70.520816434656567</v>
       </c>
+      <c r="K35" s="38">
+        <v>71.813553107833584</v>
+      </c>
     </row>
     <row r="36" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="29" t="s">
-        <v>95</v>
+      <c r="A36" s="28" t="s">
+        <v>91</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C36" s="30" t="s">
-        <v>101</v>
+        <v>86</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>97</v>
       </c>
       <c r="D36" s="2">
         <v>77.314517223351061</v>
@@ -2000,22 +2037,25 @@
       <c r="H36" s="2">
         <v>76.16207948063483</v>
       </c>
-      <c r="I36" s="39">
+      <c r="I36" s="38">
         <v>71.466218079922925</v>
       </c>
-      <c r="J36" s="39">
+      <c r="J36" s="38">
         <v>75.452380011484664</v>
       </c>
+      <c r="K36" s="38">
+        <v>74.725444681281274</v>
+      </c>
     </row>
     <row r="37" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="29" t="s">
-        <v>96</v>
+      <c r="A37" s="28" t="s">
+        <v>92</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C37" s="30" t="s">
-        <v>102</v>
+        <v>87</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>98</v>
       </c>
       <c r="D37" s="2">
         <v>77.695134204768337</v>
@@ -2032,22 +2072,25 @@
       <c r="H37" s="2">
         <v>73.787027506963781</v>
       </c>
-      <c r="I37" s="39">
+      <c r="I37" s="38">
         <v>74.357597231055067</v>
       </c>
-      <c r="J37" s="39">
+      <c r="J37" s="38">
         <v>73.964450031362844</v>
       </c>
+      <c r="K37" s="38">
+        <v>72.409661097349684</v>
+      </c>
     </row>
     <row r="38" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="29" t="s">
-        <v>97</v>
+      <c r="A38" s="28" t="s">
+        <v>93</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C38" s="30" t="s">
-        <v>103</v>
+        <v>88</v>
+      </c>
+      <c r="C38" s="29" t="s">
+        <v>99</v>
       </c>
       <c r="D38" s="2">
         <v>78.152317515623366</v>
@@ -2064,43 +2107,49 @@
       <c r="H38" s="2">
         <v>76.372726553511811</v>
       </c>
-      <c r="I38" s="39">
+      <c r="I38" s="38">
         <v>73.016879418004379</v>
       </c>
-      <c r="J38" s="39">
+      <c r="J38" s="38">
         <v>74.076691299430152</v>
       </c>
+      <c r="K38" s="38">
+        <v>72.514384944125325</v>
+      </c>
     </row>
     <row r="39" spans="1:11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="B39" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="C39" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="D39" s="8">
+      <c r="A39" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="B39" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="D39" s="7">
         <v>77.652465159687694</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E39" s="7">
         <v>78.643590497490436</v>
       </c>
-      <c r="F39" s="8">
+      <c r="F39" s="7">
         <v>78.047035618288248</v>
       </c>
-      <c r="G39" s="8">
+      <c r="G39" s="7">
         <v>77.2</v>
       </c>
-      <c r="H39" s="8">
+      <c r="H39" s="7">
         <v>73.088155829339499</v>
       </c>
-      <c r="I39" s="8">
+      <c r="I39" s="7">
         <v>73.786667018487336</v>
       </c>
-      <c r="J39" s="8">
+      <c r="J39" s="7">
         <v>70.87244746909434</v>
+      </c>
+      <c r="K39" s="7">
+        <v>74.605385456584258</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>